<commit_message>
Working on schema area changes. Switching computers, so SS.
</commit_message>
<xml_diff>
--- a/Test plan.xlsx
+++ b/Test plan.xlsx
@@ -325,7 +325,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
   <si>
     <t>Type</t>
   </si>
@@ -397,6 +397,9 @@
   </si>
   <si>
     <t>App type property</t>
+  </si>
+  <si>
+    <t>2@QZ8$IE$CaS</t>
   </si>
 </sst>
 </file>
@@ -460,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -477,10 +480,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -793,7 +799,7 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -828,22 +834,22 @@
       <c r="D2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="9"/>
+      <c r="G2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7" t="s">
+      <c r="H2" s="9"/>
+      <c r="I2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7" t="s">
+      <c r="J2" s="9"/>
+      <c r="K2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="7"/>
+      <c r="L2" s="9"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E3" s="1">
@@ -952,13 +958,13 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="E9" s="8"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="C10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>23</v>
       </c>
     </row>
@@ -995,62 +1001,65 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C20" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="I24" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>9</v>
       </c>

</xml_diff>